<commit_message>
docs(README): clarify requirement fields and add allowed values
Update README to specify allowed values, add notes about parent requirement ID and source remarks, and fix code block formatting for example report
</commit_message>
<xml_diff>
--- a/requirements.xlsx
+++ b/requirements.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="14148"/>
+    <workbookView windowWidth="20916" windowHeight="6707"/>
   </bookViews>
   <sheets>
     <sheet name="requirements" sheetId="1" r:id="rId1"/>
@@ -27,39 +27,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
-  <si>
-    <t>Title*</t>
-  </si>
-  <si>
-    <t>ProductID*</t>
-  </si>
-  <si>
-    <t>Priority*</t>
-  </si>
-  <si>
-    <t>Category*</t>
-  </si>
-  <si>
-    <t>Spec*</t>
-  </si>
-  <si>
-    <t>ParentID</t>
-  </si>
-  <si>
-    <t>Source</t>
-  </si>
-  <si>
-    <t>SourceNote</t>
-  </si>
-  <si>
-    <t>Estimate</t>
-  </si>
-  <si>
-    <t>Keywords</t>
-  </si>
-  <si>
-    <t>Verify</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
+  <si>
+    <t>标题*</t>
+  </si>
+  <si>
+    <t>产品ID*</t>
+  </si>
+  <si>
+    <t>优先级*</t>
+  </si>
+  <si>
+    <t>分类*</t>
+  </si>
+  <si>
+    <t>需求描述*</t>
+  </si>
+  <si>
+    <t>父需求ID</t>
+  </si>
+  <si>
+    <t>来源</t>
+  </si>
+  <si>
+    <t>来源备注</t>
+  </si>
+  <si>
+    <t>预计工时</t>
+  </si>
+  <si>
+    <t>关键词</t>
+  </si>
+  <si>
+    <t>验收标准</t>
   </si>
   <si>
     <t>用户登录功能</t>
@@ -71,6 +71,9 @@
     <t>实现用户登录功能，支持账号密码登录</t>
   </si>
   <si>
+    <t>market</t>
+  </si>
+  <si>
     <t>登录成功后跳转到首页</t>
   </si>
   <si>
@@ -83,7 +86,7 @@
     <t>1. 邮箱验证码验证</t>
   </si>
   <si>
-    <t>客户需求</t>
+    <t>customer</t>
   </si>
   <si>
     <t>产品经理确认</t>
@@ -95,7 +98,16 @@
     <t>2. 密码强度检查</t>
   </si>
   <si>
+    <t>po</t>
+  </si>
+  <si>
     <t>3. 用户协议确认</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>客户需求ID 62384</t>
   </si>
 </sst>
 </file>
@@ -1250,8 +1262,8 @@
   <sheetPr/>
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="14.4" outlineLevelRow="4"/>
@@ -1319,19 +1331,22 @@
       <c r="E2" t="s">
         <v>13</v>
       </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
       <c r="H2">
         <v>2.5</v>
       </c>
       <c r="J2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B3">
         <v>7</v>
@@ -1343,30 +1358,30 @@
         <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I3">
         <v>4</v>
       </c>
       <c r="J3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B4">
         <v>7</v>
@@ -1378,15 +1393,18 @@
         <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="G4" t="s">
+        <v>23</v>
       </c>
       <c r="K4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B5">
         <v>7</v>
@@ -1398,10 +1416,16 @@
         <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>22</v>
+        <v>24</v>
+      </c>
+      <c r="G5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" t="s">
+        <v>26</v>
       </c>
       <c r="K5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>